<commit_message>
Completed Bajaj insurance with proper function routing according to different submodel type
</commit_message>
<xml_diff>
--- a/Bajaj/Extracted_Bajaj_Excel/bajaj_output.xlsx
+++ b/Bajaj/Extracted_Bajaj_Excel/bajaj_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE27"/>
+  <dimension ref="A1:AE32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -598,27 +598,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>OG-23-1901-1806-00054682</t>
+          <t>OG-23-1901-1802-00035158</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ROSHAN LAL</t>
+          <t>JITENDRA KHATREE</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t> </t>
+          <t>9302583788</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>RAJRAJ0327@GMAIL.COM</t>
+          <t>deepakkochar11@gmail.com</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>VPO, KHOTHRAN,SBS NAGAR, ,, PHAGWARA - 144632</t>
+          <t>685, DWARKAPURI
+, , INDORE, MADHYA PRADESH-452001</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -628,67 +629,67 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2023/03/19</t>
+          <t>2023/03/20</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2024/03/18</t>
+          <t>2024/03/19</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>PB32R8492</t>
+          <t>MP09MZ9911</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>PB32</t>
+          <t>MP09</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>50</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2014/06/01</t>
+          <t>2010/04/01</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>HEROMOTOCORP</t>
+          <t>HEROHONDA</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>SPLENDORPLUS</t>
+          <t>PASSIONPLUS</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>CASTWHEELKICKSTART</t>
+          <t>ALLOYKICKDRUM</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>PETROL</t>
+          <t>Petrol</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>HA10EJEHD45926</t>
+          <t>HA10EBA9C00789</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>MBLHA10AMEHD24703</t>
+          <t>MBLHA10EGA9C00200</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -703,42 +704,42 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Go Digit General Insurance LimitedPrevious Policy N</t>
+          <t>National Insurance Company Limited</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>D059362942/1203022</t>
+          <t>390101231216200990126</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>2023/03/12</t>
+          <t>2023/03/16</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>17,218.00</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>225.00</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>714.00</t>
+          <t>1,045.00</t>
         </is>
       </c>
       <c r="AC2" t="n">
-        <v>714</v>
+        <v>1270</v>
       </c>
       <c r="AD2" t="n">
-        <v>129</v>
+        <v>229</v>
       </c>
       <c r="AE2" t="n">
-        <v>843</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="3">
@@ -749,27 +750,28 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>OG-23-1901-1806-00054683</t>
+          <t>OG-23-1901-1802-00035160</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>RATHOD KANUBHAI MALDEBHAI</t>
+          <t>JAY DHARMENDRA BHAI KALIYA</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t> </t>
+          <t>9737067941</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>USHARTO123@GMAIL.COM</t>
+          <t>GRIVAFIN@GMAIL.COM</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>BLOCK NO 6 SHRE RAM NAGAR, NR RAMESH PAN,CHHAYA, ,, PORBANDAR -360575</t>
+          <t>HINGLAJ NAGAR, THALTEJ
+, , AHMEDABAD, GUJARAT-380059</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -779,22 +781,22 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2023/03/19</t>
+          <t>2023/03/20</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2024/03/18</t>
+          <t>2024/03/19</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>GJ32F7313</t>
+          <t>GJ27CB5678</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>GJ32</t>
+          <t>GJ27</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -804,22 +806,22 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2017/09/01</t>
+          <t>2017/12/01</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>KTM</t>
+          <t>HONDA</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>CBHORNET</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>RC</t>
+          <t>160RSTD</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -829,17 +831,17 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>PETROL</t>
+          <t>Petrol</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>790697933</t>
+          <t>KC23E84002540</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>MD2JYCYD3HC081666</t>
+          <t>ME4KC239DH8001643</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -849,7 +851,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>163</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
@@ -864,17 +866,17 @@
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2001/01/01</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>40,000.00</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>870.00</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
@@ -883,13 +885,13 @@
         </is>
       </c>
       <c r="AC3" t="n">
-        <v>1366</v>
+        <v>2236</v>
       </c>
       <c r="AD3" t="n">
-        <v>246</v>
+        <v>402</v>
       </c>
       <c r="AE3" t="n">
-        <v>1612</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="4">
@@ -900,97 +902,98 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>OG-25-1901-1806-00024041</t>
+          <t>OG-23-1901-1802-00035163</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>RAJESHBHAI JAYRAM RATHOD</t>
+          <t>SUBE SINGH</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t> </t>
+          <t>9773770573</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>vachhanitushar1@gmail.com</t>
+          <t>RAJ958297K@GMAIL.COM</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>AT, PLOT NO 66 H NO 3186 SHRI KRISHNA NIVAS,NR PARK SOCIETY, ,, SIL-VASSA - 396230</t>
+          <t>E 35, SHAKURPUR JJ COLONY,DELHI
+, , NORTH WEST DELHI, DELHI-110034</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2024/07/08</t>
+          <t>2023/03/17</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2024/07/10</t>
+          <t>2023/03/20</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2025/07/09</t>
+          <t>2024/03/19</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>DN09H8163</t>
+          <t>DL08SBW8606</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>DN09</t>
+          <t>DL08</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>25</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2012/07/01</t>
+          <t>2016/11/01</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>HONDA</t>
+          <t>BAJAJ</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>SHINE</t>
+          <t>V15</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>SELFDRUM&amp;ALLOY</t>
+          <t>ELECTRICSTARTALLOYWHEELFR.DISC</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>PETROL</t>
+          <t>Petrol</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>JC36E7118055</t>
+          <t>JHZRGC42802</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>ME4JC36JFC7078793</t>
+          <t>MD2A74BZ5GRC42417</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -1000,47 +1003,47 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>150</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Go Digit General Insurance Limited</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t> </t>
+          <t>d058766057</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2023/03/13</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>30,420.00</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>771.00</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>714.00</t>
+          <t>1,045.00</t>
         </is>
       </c>
       <c r="AC4" t="n">
-        <v>714</v>
+        <v>1816</v>
       </c>
       <c r="AD4" t="n">
-        <v>129</v>
+        <v>327</v>
       </c>
       <c r="AE4" t="n">
-        <v>843</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="5">
@@ -1051,97 +1054,98 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>OG-25-1901-1806-00024045</t>
+          <t>OG-23-1901-1802-00035167</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ALVIN J DSOUZA</t>
+          <t>JAGAN RAJENDIRAN</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t> </t>
+          <t>9790823348</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>aasimwaliley99@gmail.com</t>
+          <t>jagan94.rajendiran@gmail.com</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>RM NO B-23 SAI VIHAR CHS NR CHANNAL, UPAVAN SAI NGR,PANVEL, ,,RAIGAD - 410206</t>
+          <t>A, A
+, , CHENNAI, TAMIL NADU-600041</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2024/07/08</t>
+          <t>2023/03/17</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2024/07/10</t>
+          <t>2023/03/18</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2025/07/09</t>
+          <t>2024/03/17</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>MH04JD0350</t>
+          <t>TN22BQ5526</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>MH04</t>
+          <t>TN22</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>50</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2017/07/01</t>
+          <t>2011/01/01</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>ROYALENFIELD</t>
+          <t>TVS</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>CLASSIC350</t>
+          <t>APACHERTR160</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>HALCYONGREENBSVI</t>
+          <t>EFIRRDISK</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2011</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>PETROL</t>
+          <t>Petrol</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>U3S5C1HE059826</t>
+          <t>OE4AB2232958</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>ME3U3S5C1HE894809</t>
+          <t>MD634KE48B2A65190</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -1151,47 +1155,47 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>349</t>
+          <t>160</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t> </t>
+          <t>ICICI Lombard General Insurance Company Limited</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t> </t>
+          <t>242633470</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2023/03/17</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>23,731.00</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>225.00</t>
         </is>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>1,316.00</t>
+          <t>1,366.00</t>
         </is>
       </c>
       <c r="AC5" t="n">
-        <v>1316</v>
+        <v>1591</v>
       </c>
       <c r="AD5" t="n">
-        <v>118</v>
+        <v>286</v>
       </c>
       <c r="AE5" t="n">
-        <v>1434</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="6">
@@ -1202,52 +1206,53 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>OG-25-1901-1806-00024046</t>
+          <t>OG-23-1901-1802-00035170</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>M SUNIL KUMAR</t>
+          <t>SHABAZ KHAN</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t> </t>
+          <t>7898443444</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>srinupenumalli@gmail.com</t>
+          <t>HINA.SSPLC@GMAIL.COM</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>S/O LAKSHMANA RAO,41-1/2-36,3RD LINE, DWARAKANAGAR,KRISHNALANKA, ,, VIJAYAWADA - 520013</t>
+          <t>HNO1, B/H-VIVEKANAND ASHRAM IDGAH,BHATHA RAIPUR
+, , RAIPUR, CHATTISGARH-492001</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2024/07/08</t>
+          <t>2023/03/18</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2024/07/10</t>
+          <t>2023/03/20</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2025/07/09</t>
+          <t>2024/03/19</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>AP16AV2322</t>
+          <t>CG04LC8220</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>AP16</t>
+          <t>CG04</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1257,42 +1262,42 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2008/05/01</t>
+          <t>2016/01/01</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>BAJAJ</t>
+          <t>HEROMOTOCORP</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>DISCOVER135DTSI</t>
+          <t>SPLENDORPLUS</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>ELECTRICSTART</t>
+          <t>CASTWHEELSELFSTART</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2008</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>PETROL</t>
+          <t>Petrol</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>JNGBPJ23133</t>
+          <t>HA10ERFHM76445</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>MD2DSJNZZPCJ12887</t>
+          <t>MBLHA10CGFHM14537</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -1302,7 +1307,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>100</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
@@ -1317,32 +1322,32 @@
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2001/01/01</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>22,975.00</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>329.00</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>714.00</t>
+          <t>1,045.00</t>
         </is>
       </c>
       <c r="AC6" t="n">
-        <v>714</v>
+        <v>1374</v>
       </c>
       <c r="AD6" t="n">
-        <v>129</v>
+        <v>247</v>
       </c>
       <c r="AE6" t="n">
-        <v>843</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="7">
@@ -1353,12 +1358,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>OG-25-1901-1806-00024047</t>
+          <t>OG-23-1901-1806-00054682</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>BALAJI PANDURANG SHINDE</t>
+          <t>ROSHAN LAL</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1368,37 +1373,37 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>mkonade@gmail.com</t>
+          <t>RAJRAJ0327@GMAIL.COM</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>AP, SOLAPUR,SOLAPUR, ,, SOLAPUR - 413004</t>
+          <t>VPO, KHOTHRAN,SBS NAGAR, ,, PHAGWARA - 144632</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2024/07/08</t>
+          <t>2023/03/17</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2024/07/10</t>
+          <t>2023/03/19</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2025/07/09</t>
+          <t>2024/03/18</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>MH13AW9718</t>
+          <t>PB32R8492</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>MH13</t>
+          <t>PB32</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -1408,7 +1413,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2010/12/01</t>
+          <t>2014/06/01</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -1418,17 +1423,17 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>PASSIONPRO</t>
+          <t>SPLENDORPLUS</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>DISCBREAKSELFSTARTBSVI</t>
+          <t>CASTWHEELKICKSTART</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1438,12 +1443,12 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>HA10EDAGL37805</t>
+          <t>HA10EJEHD45926</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>MBLHA10AKAGL04086</t>
+          <t>MBLHA10AMEHD24703</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -1453,22 +1458,22 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>100</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Go Digit General Insurance LimitedPrevious Policy N</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t> </t>
+          <t>D059362942/1203022</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2023/03/12</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
@@ -1483,17 +1488,17 @@
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>664.00</t>
+          <t>714.00</t>
         </is>
       </c>
       <c r="AC7" t="n">
-        <v>664</v>
+        <v>714</v>
       </c>
       <c r="AD7" t="n">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="AE7" t="n">
-        <v>724</v>
+        <v>843</v>
       </c>
     </row>
     <row r="8">
@@ -1504,12 +1509,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>OG-25-1901-1806-00024049</t>
+          <t>OG-23-1901-1806-00054683</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>DALAL BIMALBHAI RAJNIKANTC</t>
+          <t>RATHOD KANUBHAI MALDEBHAI</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1519,37 +1524,37 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>BELAPRAJAPATI17@GMAIL.COM</t>
+          <t>USHARTO123@GMAIL.COM</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>C-3 KENDRIYA KARMACHARI NAGAR, INDIRA NAGAR ROAD NADIAD,DIKHEDA, ,, CHANDKHEDA - 387002</t>
+          <t>BLOCK NO 6 SHRE RAM NAGAR, NR RAMESH PAN,CHHAYA, ,, PORBANDAR -360575</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2024/07/08</t>
+          <t>2023/03/17</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2024/07/10</t>
+          <t>2023/03/19</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2025/07/09</t>
+          <t>2024/03/18</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>GJ07CG3023</t>
+          <t>GJ32F7313</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>GJ07</t>
+          <t>GJ32</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1559,27 +1564,27 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2016/06/01</t>
+          <t>2017/09/01</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>HEROMOTOCORP</t>
+          <t>KTM</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>SPLENDORPLUS</t>
+          <t>200</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>CASTWHEELSELFSTART</t>
+          <t>RC</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1589,12 +1594,12 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>HA10ERGHE46330</t>
+          <t>790697933</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>MBLHA10CGGHE44224</t>
+          <t>MD2JYCYD3HC081666</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1604,7 +1609,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>200</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -1634,17 +1639,17 @@
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>1,157.00</t>
+          <t>1,366.00</t>
         </is>
       </c>
       <c r="AC8" t="n">
-        <v>1157</v>
+        <v>1366</v>
       </c>
       <c r="AD8" t="n">
-        <v>208</v>
+        <v>246</v>
       </c>
       <c r="AE8" t="n">
-        <v>1365</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="9">
@@ -1655,12 +1660,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>OG-25-1901-1806-00024050</t>
+          <t>OG-25-1901-1806-00024041</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>AMIR KARIM KHAN</t>
+          <t>RAJESHBHAI JAYRAM RATHOD</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1670,12 +1675,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>TAYABSHAIKH95@GMAIL.COM</t>
+          <t>vachhanitushar1@gmail.com</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>AP HABIB PURA, PARLI TQ PARLI DIST BEED, ,, BEED - 431515</t>
+          <t>AT, PLOT NO 66 H NO 3186 SHRI KRISHNA NIVAS,NR PARK SOCIETY, ,, SIL-VASSA - 396230</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1695,12 +1700,12 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>MH20BU8859</t>
+          <t>DN09H8163</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>MH20</t>
+          <t>DN09</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1710,27 +1715,27 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>2010/10/01</t>
+          <t>2012/07/01</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>HEROMOTOCORP</t>
+          <t>HONDA</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>SPLENDORPLUS</t>
+          <t>SHINE</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>I3SFISELFSTARTCASTWHEELBSVI</t>
+          <t>SELFDRUM&amp;ALLOY</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1740,12 +1745,12 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>HA10EFAHH08644</t>
+          <t>JC36E7118055</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>MBLHA10EZAHH43965</t>
+          <t>ME4JC36JFC7078793</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -1755,7 +1760,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>125</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -1785,33 +1790,33 @@
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>1,045.00</t>
+          <t>714.00</t>
         </is>
       </c>
       <c r="AC9" t="n">
-        <v>1045</v>
+        <v>714</v>
       </c>
       <c r="AD9" t="n">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="AE9" t="n">
-        <v>1139</v>
+        <v>843</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Pcv</t>
+          <t>Two wheeler</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>OG-19-1901-1803-00005678</t>
+          <t>OG-25-1901-1806-00024045</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RAMAKANT S YADAV</t>
+          <t>ALVIN J DSOUZA</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1821,148 +1826,148 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>SATISHG527@GMAIL.COM</t>
+          <t>aasimwaliley99@gmail.com</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>RAMAKANT CHAUDHARI CHAWL, HAWAI PADA GAURAIPADA VASAI E, ,,VASAI - 401208</t>
+          <t>RM NO B-23 SAI VIHAR CHS NR CHANNAL, UPAVAN SAI NGR,PANVEL, ,,RAIGAD - 410206</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2018/12/03</t>
+          <t>2024/07/08</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2018/12/05</t>
+          <t>2024/07/10</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2019/12/04</t>
+          <t>2025/07/09</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>MH48N5018</t>
+          <t>MH04JD0350</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>MH48</t>
+          <t>MH04</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2017/07/01</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>BAJAJ</t>
+          <t>ROYALENFIELD</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>REARENGINEPETROL</t>
+          <t>CLASSIC350</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>AUTORIKSHAW2STROKE</t>
+          <t>HALCYONGREENBSVI</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t> </t>
+          <t>PETROL</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>H69887`</t>
+          <t>U3S5C1HE059826</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>H21946</t>
+          <t>ME3U3S5C1HE894809</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>349</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>Tata AIG General Insurance Company Limited</t>
+          <t> </t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>0156499274</t>
+          <t> </t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>2018/12/04</t>
+          <t> </t>
         </is>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>75600</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>620</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>6918</t>
+          <t>1,316.00</t>
         </is>
       </c>
       <c r="AC10" t="n">
-        <v>7538</v>
+        <v>1316</v>
       </c>
       <c r="AD10" t="n">
-        <v>1356</v>
+        <v>118</v>
       </c>
       <c r="AE10" t="n">
-        <v>8894</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Gcv</t>
+          <t>Two wheeler</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>OG-19-1901-1803-00006583</t>
+          <t>OG-25-1901-1806-00024046</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>RAMBAHADUR SHAMBAHADUR DHOBI</t>
+          <t>M SUNIL KUMAR</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1972,82 +1977,82 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>dkinvestment9@gmail.com</t>
+          <t>srinupenumalli@gmail.com</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>TA-1 SEGHNA 11 SANJAY NAGAR, ZOPADPATTI VIBHAG B ASUNAVALI,AGYARI MARG, ,, MUMBAI - 400016</t>
+          <t>S/O LAKSHMANA RAO,41-1/2-36,3RD LINE, DWARAKANAGAR,KRISHNALANKA, ,, VIJAYAWADA - 520013</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2018/12/28</t>
+          <t>2024/07/08</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2018/12/29</t>
+          <t>2024/07/10</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2019/12/28</t>
+          <t>2025/07/09</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>MH01LA9677</t>
+          <t>AP16AV2322</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>MH01</t>
+          <t>AP16</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2008/05/01</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>TATA</t>
+          <t>BAJAJ</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>ACEHT</t>
+          <t>DISCOVER135DTSI</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>CLOSEDBODY</t>
+          <t>ELECTRICSTART</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2008</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t> </t>
+          <t>PETROL</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>JXYSJ7868</t>
+          <t>JNGBPJ23133</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>CZJ82324</t>
+          <t>MD2DSJNZZPCJ12887</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
@@ -2057,63 +2062,63 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>135</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>SBI General Insurance Company Limited</t>
+          <t> </t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>1360017-04</t>
+          <t> </t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>2018/12/28</t>
+          <t> </t>
         </is>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>207684</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>559</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>15140</t>
+          <t>714.00</t>
         </is>
       </c>
       <c r="AC11" t="n">
-        <v>15699</v>
+        <v>714</v>
       </c>
       <c r="AD11" t="n">
-        <v>2826</v>
+        <v>129</v>
       </c>
       <c r="AE11" t="n">
-        <v>18525</v>
+        <v>843</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Gcv</t>
+          <t>Two wheeler</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>OG-19-1901-1803-00008864</t>
+          <t>OG-25-1901-1806-00024047</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>SHUBHAM PRINTS LLP</t>
+          <t>BALAJI PANDURANG SHINDE</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2123,82 +2128,82 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>abhinaventerprises2009@gmail.com</t>
+          <t>mkonade@gmail.com</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>UNIT NO 110-111-A-1, 1ST FLR, SHAH AND NAHAR IND ESTATE S J,MARGLOWER PAREL, ,, MUMBAI - 400013</t>
+          <t>AP, SOLAPUR,SOLAPUR, ,, SOLAPUR - 413004</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2019/02/14</t>
+          <t>2024/07/08</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2019/02/18</t>
+          <t>2024/07/10</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2020/02/17</t>
+          <t>2025/07/09</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>MH01BR0783</t>
+          <t>MH13AW9718</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>MH01</t>
+          <t>MH13</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2010/12/01</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>TATA</t>
+          <t>HEROMOTOCORP</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>ACEDICOR</t>
+          <t>PASSIONPRO</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>HALFDECKLOADBODYGVW1770</t>
+          <t>DISCBREAKSELFSTARTBSVI</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t> </t>
+          <t>PETROL</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>LTDICRAIL05MVYSC9620</t>
+          <t>HA10EDAGL37805</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>MAT445404EVP55344</t>
+          <t>MBLHA10AKAGL04086</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
@@ -2208,63 +2213,63 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>110</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>IFFCO Tokio General Insurance Company Limited.</t>
+          <t> </t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>25420628</t>
+          <t> </t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>2019/02/17</t>
+          <t> </t>
         </is>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>240706</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>948</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>14390</t>
+          <t>664.00</t>
         </is>
       </c>
       <c r="AC12" t="n">
-        <v>15338</v>
+        <v>664</v>
       </c>
       <c r="AD12" t="n">
-        <v>1896</v>
+        <v>60</v>
       </c>
       <c r="AE12" t="n">
-        <v>17234</v>
+        <v>724</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Pcv</t>
+          <t>Two wheeler</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>OG-19-1901-1831-00004091</t>
+          <t>OG-25-1901-1806-00024049</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DILAVARBHAI KASAMBHAI MEMON</t>
+          <t>DALAL BIMALBHAI RAJNIKANTC</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2274,37 +2279,37 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>jasminins33@gmail.com</t>
+          <t>BELAPRAJAPATI17@GMAIL.COM</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>DEESA, TA DEESA,BANASKANTHA, ,, BANASKANTHA - 385535</t>
+          <t>C-3 KENDRIYA KARMACHARI NAGAR, INDIRA NAGAR ROAD NADIAD,DIKHEDA, ,, CHANDKHEDA - 387002</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2018/11/03</t>
+          <t>2024/07/08</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2018/11/03</t>
+          <t>2024/07/10</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2019/11/02</t>
+          <t>2025/07/09</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>GJ08Y2531</t>
+          <t>GJ07CG3023</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>GJ08</t>
+          <t>GJ07</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -2314,52 +2319,52 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2016/06/01</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>MARUTI</t>
+          <t>HEROMOTOCORP</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>EECO</t>
+          <t>SPLENDORPLUS</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>(4+1)STRCNG</t>
+          <t>CASTWHEELSELFSTART</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t> </t>
+          <t>PETROL</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>356987</t>
+          <t>HA10ERGHE46330</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>38089</t>
+          <t>MBLHA10CGGHE44224</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>1196</t>
+          <t>100</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
@@ -2389,33 +2394,33 @@
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>11527</t>
+          <t>1,157.00</t>
         </is>
       </c>
       <c r="AC13" t="n">
-        <v>11527</v>
+        <v>1157</v>
       </c>
       <c r="AD13" t="n">
-        <v>2075</v>
+        <v>208</v>
       </c>
       <c r="AE13" t="n">
-        <v>13602</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Pcv</t>
+          <t>Two wheeler</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>OG-19-1901-1831-00004251</t>
+          <t>OG-25-1901-1806-00024050</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>JAY KHODIYAR TRAVELS</t>
+          <t>AMIR KARIM KHAN</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2425,37 +2430,37 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>amishdedhia76@gmail.com</t>
+          <t>TAYABSHAIKH95@GMAIL.COM</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>ROOM NO 2 GAON DEVI COMP NEAR, VISHNU MANDIR MAHAJAN-WADI,GAVTHAN MIRAROAD, ,, THANE - 401107</t>
+          <t>AP HABIB PURA, PARLI TQ PARLI DIST BEED, ,, BEED - 431515</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2018/11/19</t>
+          <t>2024/07/08</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2018/11/19</t>
+          <t>2024/07/10</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2019/11/18</t>
+          <t>2025/07/09</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>MH04HN2497</t>
+          <t>MH20BU8859</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>MH04</t>
+          <t>MH20</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -2465,52 +2470,52 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2010/10/01</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>MARUTI</t>
+          <t>HEROMOTOCORP</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>EECO</t>
+          <t>SPLENDORPLUS</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>(6+1)STRWITHA/C+HTRCNG</t>
+          <t>I3SFISELFSTARTCASTWHEELBSVI</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>PETROL</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>474211</t>
+          <t>HA10EFAHH08644</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>497559</t>
+          <t>MBLHA10EZAHH43965</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>1196</t>
+          <t>100</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
@@ -2540,33 +2545,33 @@
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>12487</t>
+          <t>1,045.00</t>
         </is>
       </c>
       <c r="AC14" t="n">
-        <v>12487</v>
+        <v>1045</v>
       </c>
       <c r="AD14" t="n">
-        <v>2248</v>
+        <v>94</v>
       </c>
       <c r="AE14" t="n">
-        <v>14735</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Gcv</t>
+          <t>Pcv</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>OG-19-1901-1831-00004270</t>
+          <t>OG-19-1901-1803-00005678</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>SHIRISH SHIVAJI ANDHALE</t>
+          <t>RAMAKANT S YADAV</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -2576,32 +2581,32 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>amishdedhia76@gmail.com</t>
+          <t>SATISHG527@GMAIL.COM</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>R NO 601 RAVI BLDG JAGJID, COMPLEX MIRAROAD EAST, ,, THANE - 401107</t>
+          <t>RAMAKANT CHAUDHARI CHAWL, HAWAI PADA GAURAIPADA VASAI E, ,,VASAI - 401208</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2018/11/21</t>
+          <t>2018/12/03</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2018/11/21</t>
+          <t>2018/12/05</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2019/11/20</t>
+          <t>2019/12/04</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>MH48T3478</t>
+          <t>MH48N5018</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -2611,7 +2616,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>35</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -2621,22 +2626,22 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>TATA</t>
+          <t>BAJAJ</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>LPT1109EX</t>
+          <t>REARENGINEPETROL</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>HIGHDECKLOADBODY(GVW12900)</t>
+          <t>AUTORIKSHAW2STROKE</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -2646,62 +2651,62 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>840870</t>
+          <t>H69887`</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>7H25063</t>
+          <t>H21946</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>1196</t>
+          <t>150</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Tata AIG General Insurance Company Limited</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t> </t>
+          <t>0156499274</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2018/12/04</t>
         </is>
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>75600</t>
         </is>
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>620</t>
         </is>
       </c>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>32417</t>
+          <t>6918</t>
         </is>
       </c>
       <c r="AC15" t="n">
-        <v>32417</v>
+        <v>7538</v>
       </c>
       <c r="AD15" t="n">
-        <v>5836</v>
+        <v>1356</v>
       </c>
       <c r="AE15" t="n">
-        <v>38253</v>
+        <v>8894</v>
       </c>
     </row>
     <row r="16">
@@ -2712,12 +2717,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>OG-19-1901-1831-00004272</t>
+          <t>OG-19-1901-1803-00006583</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>AJAY BALARRAM PATIL</t>
+          <t>RAMBAHADUR SHAMBAHADUR DHOBI</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -2727,42 +2732,42 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>CARSPOTINSURANCE@GMAIL.COM</t>
+          <t>dkinvestment9@gmail.com</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>AZAD NAGAR SAMBHAJI NAGAR, VASAI E, ,, VASAI - 401202</t>
+          <t>TA-1 SEGHNA 11 SANJAY NAGAR, ZOPADPATTI VIBHAG B ASUNAVALI,AGYARI MARG, ,, MUMBAI - 400016</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2018/11/21</t>
+          <t>2018/12/28</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2018/11/21</t>
+          <t>2018/12/29</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2019/11/20</t>
+          <t>2019/12/28</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>MH04CG3858</t>
+          <t>MH01LA9677</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>MH04</t>
+          <t>MH01</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>50</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -2777,17 +2782,17 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>SFC407HT</t>
+          <t>ACEHT</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>HALFDECKLOADBODY</t>
+          <t>CLOSEDBODY</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -2797,12 +2802,12 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>15249</t>
+          <t>JXYSJ7868</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>A04443</t>
+          <t>CZJ82324</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
@@ -2812,47 +2817,47 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>1196</t>
+          <t>150</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t> </t>
+          <t>SBI General Insurance Company Limited</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t> </t>
+          <t>1360017-04</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2018/12/28</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>207684</t>
         </is>
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>559</t>
         </is>
       </c>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>15190</t>
+          <t>15140</t>
         </is>
       </c>
       <c r="AC16" t="n">
-        <v>15190</v>
+        <v>15699</v>
       </c>
       <c r="AD16" t="n">
-        <v>2734</v>
+        <v>2826</v>
       </c>
       <c r="AE16" t="n">
-        <v>17924</v>
+        <v>18525</v>
       </c>
     </row>
     <row r="17">
@@ -2863,12 +2868,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>OG-19-1901-1831-00004280</t>
+          <t>OG-19-1901-1803-00008864</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>PRAKASHBHAI MOHANBHAI PRAJAPATI</t>
+          <t>SHUBHAM PRINTS LLP</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2878,42 +2883,42 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>JAYESHGUPTA.INSURANCE@gmail.com</t>
+          <t>abhinaventerprises2009@gmail.com</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>A/9 SHYAM VIHAR BUNGLOW-2, RADHANPUR ROAD,MAHESANA-74, ,, MEH-SANA - 384001</t>
+          <t>UNIT NO 110-111-A-1, 1ST FLR, SHAH AND NAHAR IND ESTATE S J,MARGLOWER PAREL, ,, MUMBAI - 400013</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2018/11/22</t>
+          <t>2019/02/14</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2018/11/22</t>
+          <t>2019/02/18</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2019/11/21</t>
+          <t>2020/02/17</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>GJ18U6887</t>
+          <t>MH01BR0783</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>GJ18</t>
+          <t>MH01</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>25</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -2928,17 +2933,17 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>SE1613</t>
+          <t>ACEDICOR</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>HALFDECKLOADBODY</t>
+          <t>HALFDECKLOADBODYGVW1770</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -2948,12 +2953,12 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>133291</t>
+          <t>LTDICRAIL05MVYSC9620</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>749083</t>
+          <t>MAT445404EVP55344</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
@@ -2963,47 +2968,47 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>1196</t>
+          <t>150</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t> </t>
+          <t>IFFCO Tokio General Insurance Company Limited.</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t> </t>
+          <t>25420628</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2019/02/17</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>240706</t>
         </is>
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>948</t>
         </is>
       </c>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>33167</t>
+          <t>14390</t>
         </is>
       </c>
       <c r="AC17" t="n">
-        <v>33167</v>
+        <v>15338</v>
       </c>
       <c r="AD17" t="n">
-        <v>5970</v>
+        <v>1896</v>
       </c>
       <c r="AE17" t="n">
-        <v>39137</v>
+        <v>17234</v>
       </c>
     </row>
     <row r="18">
@@ -3014,12 +3019,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>OG-19-1901-1831-00004418</t>
+          <t>OG-19-1901-1831-00004091</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>BAJARANG TOURS AND TRAVELS</t>
+          <t>DILAVARBHAI KASAMBHAI MEMON</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -3029,37 +3034,37 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>INSURANCEPOINTPUNE@GMAIL.COM</t>
+          <t>jasminins33@gmail.com</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>PROP BAJARANG BHOSLE, ROOM NO-405 THALE APTS PURNA,VILLAGETAL-BHIWANDI, ,, THANE - 421302</t>
+          <t>DEESA, TA DEESA,BANASKANTHA, ,, BANASKANTHA - 385535</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2018/12/01</t>
+          <t>2018/11/03</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2018/12/01</t>
+          <t>2018/11/03</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2019/11/30</t>
+          <t>2019/11/02</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>MH04GD6165</t>
+          <t>GJ08Y2531</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>MH04</t>
+          <t>GJ08</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -3074,17 +3079,17 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>HYUNDAI</t>
+          <t>MARUTI</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>XCENT</t>
+          <t>EECO</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>1.2U2CRDI5SPEEDMANUALS(4+1)</t>
+          <t>(4+1)STRCNG</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
@@ -3099,12 +3104,12 @@
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>M406688</t>
+          <t>356987</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>M136172</t>
+          <t>38089</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
@@ -3114,7 +3119,7 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>1186</t>
+          <t>1196</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
@@ -3144,17 +3149,17 @@
       </c>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>11467</t>
+          <t>11527</t>
         </is>
       </c>
       <c r="AC18" t="n">
-        <v>11467</v>
+        <v>11527</v>
       </c>
       <c r="AD18" t="n">
-        <v>2064</v>
+        <v>2075</v>
       </c>
       <c r="AE18" t="n">
-        <v>13531</v>
+        <v>13602</v>
       </c>
     </row>
     <row r="19">
@@ -3165,12 +3170,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>OG-19-1901-1831-00004467</t>
+          <t>OG-19-1901-1831-00004251</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>SITARA KHALIL AHMED KHAN</t>
+          <t>JAY KHODIYAR TRAVELS</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -3180,37 +3185,37 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>shafiquekhan@gmail.com</t>
+          <t>amishdedhia76@gmail.com</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>JAIRAJ LANE R NO 80 NAWAB, CHAWL NO. 5 MUMBAI, ,, MUMBAI - 400008</t>
+          <t>ROOM NO 2 GAON DEVI COMP NEAR, VISHNU MANDIR MAHAJAN-WADI,GAVTHAN MIRAROAD, ,, THANE - 401107</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2018/12/05</t>
+          <t>2018/11/19</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2018/12/05</t>
+          <t>2018/11/19</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2019/12/04</t>
+          <t>2019/11/18</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>MH01BM4244</t>
+          <t>MH04HN2497</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>MH01</t>
+          <t>MH04</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -3235,12 +3240,12 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>(4+1)STRCNG</t>
+          <t>(6+1)STRWITHA/C+HTRCNG</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -3250,17 +3255,17 @@
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>301576</t>
+          <t>474211</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>325440</t>
+          <t>497559</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
@@ -3295,378 +3300,375 @@
       </c>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>10577</t>
+          <t>12487</t>
         </is>
       </c>
       <c r="AC19" t="n">
-        <v>10577</v>
+        <v>12487</v>
       </c>
       <c r="AD19" t="n">
-        <v>1904</v>
+        <v>2248</v>
       </c>
       <c r="AE19" t="n">
-        <v>12481</v>
+        <v>14735</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Private Car</t>
+          <t>Gcv</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>OG-25-1901-1801-00002377</t>
+          <t>OG-19-1901-1831-00004270</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ANJALI GUPTA</t>
+          <t>SHIRISH SHIVAJI ANDHALE</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>9099005661</t>
+          <t> </t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>gupta.ankitbds@gmail.com</t>
+          <t>amishdedhia76@gmail.com</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>19 NUPUR SHREE RESIDENCY, NEAR GANESH DHAM,INDORE
-, , INDORE, MADHYA PRADESH-452016</t>
+          <t>R NO 601 RAVI BLDG JAGJID, COMPLEX MIRAROAD EAST, ,, THANE - 401107</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2024/07/17</t>
+          <t>2018/11/21</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2024/07/18</t>
+          <t>2018/11/21</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2025/07/17</t>
+          <t>2019/11/20</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>MP09CY8865</t>
+          <t>MH48T3478</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>MP09</t>
+          <t>MH48</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>2018/08/01</t>
+          <t> </t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>MARUTI</t>
+          <t>TATA</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>VITARABREZZA</t>
+          <t>LPT1109EX</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>1.2ZDIDDIS200</t>
+          <t>HIGHDECKLOADBODY(GVW12900)</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>Diesel</t>
+          <t> </t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>D13A5680510</t>
+          <t>840870</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>MA3NYFB1SJG407267</t>
+          <t>7H25063</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>1248</t>
+          <t>1196</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>ICICI Lombard General Insurance Company Limited</t>
+          <t> </t>
         </is>
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>3001/252668986/01/000</t>
+          <t> </t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>2024/07/17</t>
+          <t> </t>
         </is>
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>4,56,362.00</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>7,445.00</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>3,716.00</t>
+          <t>32417</t>
         </is>
       </c>
       <c r="AC20" t="n">
-        <v>11161</v>
+        <v>32417</v>
       </c>
       <c r="AD20" t="n">
-        <v>2009</v>
+        <v>5836</v>
       </c>
       <c r="AE20" t="n">
-        <v>13170</v>
+        <v>38253</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Private Car</t>
+          <t>Gcv</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>OG-25-1901-1801-00002379</t>
+          <t>OG-19-1901-1831-00004272</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CHANNAPPA SHIVASHANKAREPPA NIMBAL</t>
+          <t>AJAY BALARRAM PATIL</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>8317390500</t>
+          <t> </t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>hiremathsp7@gmail.com</t>
+          <t>CARSPOTINSURANCE@GMAIL.COM</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>S/O SHUVASHANKRAPPA #144, RAMESHWAR COLONY,JAMKHANDI9448035105
-, , BAGALKOT, KARNATAKA-587301</t>
+          <t>AZAD NAGAR SAMBHAJI NAGAR, VASAI E, ,, VASAI - 401202</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2024/07/17</t>
+          <t>2018/11/21</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2024/07/20</t>
+          <t>2018/11/21</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2025/07/19</t>
+          <t>2019/11/20</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>KA48M7159</t>
+          <t>MH04CG3858</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>KA48</t>
+          <t>MH04</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>2015/08/01</t>
+          <t> </t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>TOYOTA</t>
+          <t>TATA</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>INNOVA</t>
+          <t>SFC407HT</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>2.5VX(Diesel)</t>
+          <t>HALFDECKLOADBODY</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>Diesel</t>
+          <t> </t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>556590</t>
+          <t>15249</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>220715</t>
+          <t>A04443</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>2</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>2494</t>
+          <t>1196</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>Liberty general insurance limited</t>
+          <t> </t>
         </is>
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>201150021223700057600000</t>
+          <t> </t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
         <is>
-          <t>2024/07/19</t>
+          <t> </t>
         </is>
       </c>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>6,15,000.00</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>9,604.00</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>8,347.00</t>
+          <t>15190</t>
         </is>
       </c>
       <c r="AC21" t="n">
-        <v>17951</v>
+        <v>15190</v>
       </c>
       <c r="AD21" t="n">
-        <v>3231</v>
+        <v>2734</v>
       </c>
       <c r="AE21" t="n">
-        <v>21182</v>
+        <v>17924</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Private Car</t>
+          <t>Gcv</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>OG-25-1901-1801-00002380</t>
+          <t>OG-19-1901-1831-00004280</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>GIRISH J M</t>
+          <t>PRAKASHBHAI MOHANBHAI PRAJAPATI</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>7899365929</t>
+          <t> </t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>girishdkj@gmail.com</t>
+          <t>JAYESHGUPTA.INSURANCE@gmail.com</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>NO 512, 8TH MAIN ROAD 9TH CROSS,SADASHIVANAGAR
-, , BENGALURU, KARNATAKA-560080</t>
+          <t>A/9 SHYAM VIHAR BUNGLOW-2, RADHANPUR ROAD,MAHESANA-74, ,, MEH-SANA - 384001</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2024/07/17</t>
+          <t>2018/11/22</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2024/07/20</t>
+          <t>2018/11/22</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2025/07/19</t>
+          <t>2019/11/21</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>KA04MR9739</t>
+          <t>GJ18U6887</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>KA04</t>
+          <t>GJ18</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -3676,108 +3678,108 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>2016/08/01</t>
+          <t> </t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>MARUTI</t>
+          <t>TATA</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>VITARABREZZA</t>
+          <t>SE1613</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>1.2ZDIDDIS200</t>
+          <t>HALFDECKLOADBODY</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>Diesel</t>
+          <t> </t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>D13A5277803</t>
+          <t>133291</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>MA3NYFB1SGF126243</t>
+          <t>749083</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>1248</t>
+          <t>1196</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>Future Generali India Insurance Company Limited</t>
+          <t> </t>
         </is>
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>VB999570</t>
+          <t> </t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>2024/07/19</t>
+          <t> </t>
         </is>
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>3,50,000.00</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>7,582.00</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>3,797.00</t>
+          <t>33167</t>
         </is>
       </c>
       <c r="AC22" t="n">
-        <v>11379</v>
+        <v>33167</v>
       </c>
       <c r="AD22" t="n">
-        <v>2048</v>
+        <v>5970</v>
       </c>
       <c r="AE22" t="n">
-        <v>13427</v>
+        <v>39137</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Private Car</t>
+          <t>Pcv</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>OG-25-1901-1805-00000874</t>
+          <t>OG-19-1901-1831-00004418</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>JITENDRABHAI MAGANBHAI PATEL</t>
+          <t>BAJARANG TOURS AND TRAVELS</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -3787,37 +3789,37 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>mcpatel1985@gmail.com</t>
+          <t>INSURANCEPOINTPUNE@GMAIL.COM</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>AT-ANIYORKAMPA, TA-MALPUR,DIST-ARVALLI, ,, MALPUR - 383345</t>
+          <t>PROP BAJARANG BHOSLE, ROOM NO-405 THALE APTS PURNA,VILLAGETAL-BHIWANDI, ,, THANE - 421302</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2024/07/17</t>
+          <t>2018/12/01</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2024/07/20</t>
+          <t>2018/12/01</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2025/07/19</t>
+          <t>2019/11/30</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>GJ09AG3376</t>
+          <t>MH04GD6165</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>GJ09</t>
+          <t>MH04</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -3827,67 +3829,67 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>2010/05/01</t>
+          <t> </t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>MARUTI</t>
+          <t>HYUNDAI</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>RITZ</t>
+          <t>XCENT</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>LDI</t>
+          <t>1.2U2CRDI5SPEEDMANUALS(4+1)</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t> </t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>D13A1378382</t>
+          <t>M406688</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>MA3FDEB1S00164202</t>
+          <t>M136172</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>1248</t>
+          <t>1186</t>
         </is>
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>Future Generali India Insurance Company Limited</t>
+          <t> </t>
         </is>
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>VB992563</t>
+          <t> </t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>2024/07/19</t>
+          <t> </t>
         </is>
       </c>
       <c r="Z23" t="inlineStr">
@@ -3902,33 +3904,33 @@
       </c>
       <c r="AB23" t="inlineStr">
         <is>
-          <t>3,922.00</t>
+          <t>11467</t>
         </is>
       </c>
       <c r="AC23" t="n">
-        <v>3922</v>
+        <v>11467</v>
       </c>
       <c r="AD23" t="n">
-        <v>706</v>
+        <v>2064</v>
       </c>
       <c r="AE23" t="n">
-        <v>4628</v>
+        <v>13531</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Private Car</t>
+          <t>Pcv</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>OG-25-1901-1805-00000875</t>
+          <t>OG-19-1901-1831-00004467</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>SARPARIYA NARENDRA VASANTDAS</t>
+          <t>SITARA KHALIL AHMED KHAN</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -3938,37 +3940,37 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>KAPILNIMAVAT93@GMAIL.COM</t>
+          <t>shafiquekhan@gmail.com</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>AT, NEAR NEW BUS STAND,UPLETA, ,, RAJKOT - 360490</t>
+          <t>JAIRAJ LANE R NO 80 NAWAB, CHAWL NO. 5 MUMBAI, ,, MUMBAI - 400008</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2024/07/17</t>
+          <t>2018/12/05</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2024/07/19</t>
+          <t>2018/12/05</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2025/07/18</t>
+          <t>2019/12/04</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>GJ25J4484</t>
+          <t>MH01BM4244</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>GJ25</t>
+          <t>MH01</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -3978,7 +3980,7 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>2015/11/01</t>
+          <t> </t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -3988,42 +3990,42 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>BALENONEW</t>
+          <t>EECO</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>ALPHADIESEL</t>
+          <t>(4+1)STRCNG</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t> </t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>D13A2705399</t>
+          <t>301576</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>MA3EWB62SFK104130</t>
+          <t>325440</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>1248</t>
+          <t>1196</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
@@ -4053,17 +4055,17 @@
       </c>
       <c r="AB24" t="inlineStr">
         <is>
-          <t>4,047.00</t>
+          <t>10577</t>
         </is>
       </c>
       <c r="AC24" t="n">
-        <v>4047</v>
+        <v>10577</v>
       </c>
       <c r="AD24" t="n">
-        <v>728</v>
+        <v>1904</v>
       </c>
       <c r="AE24" t="n">
-        <v>4775</v>
+        <v>12481</v>
       </c>
     </row>
     <row r="25">
@@ -4074,27 +4076,28 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>OG-25-1901-1805-00000876</t>
+          <t>OG-25-1901-1801-00002377</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>JAYRAJBHAI AMKUBHAI MANJARIYA</t>
+          <t>ANJALI GUPTA</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t> </t>
+          <t>9099005661</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>mayur_auto02@yahoo.in</t>
+          <t>gupta.ankitbds@gmail.com</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>00, DANEV SOCIETY HANUMAN MANDIR PASE,AT-CHALALA TAL-DHARIDIST-, ,, AMRELI - 365630</t>
+          <t>19 NUPUR SHREE RESIDENCY, NEAR GANESH DHAM,INDORE
+, , INDORE, MADHYA PRADESH-452016</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -4104,67 +4107,67 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2024/07/19</t>
+          <t>2024/07/18</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2025/07/18</t>
+          <t>2025/07/17</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>GJ14AK7773</t>
+          <t>MP09CY8865</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>GJ14</t>
+          <t>MP09</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>20</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>2016/11/01</t>
+          <t>2018/08/01</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>HYUNDAI</t>
+          <t>MARUTI</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>i20</t>
+          <t>VITARABREZZA</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>ELITE1.4ASTAU2CRDI6SPEEDMANUALDIESEL</t>
+          <t>1.2ZDIDDIS200</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>Diesel</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>D4FCGM057507</t>
+          <t>D13A5680510</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>MALBM51RLGM237900</t>
+          <t>MA3NYFB1SJG407267</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
@@ -4174,47 +4177,47 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>1396</t>
+          <t>1248</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
         <is>
-          <t> </t>
+          <t>ICICI Lombard General Insurance Company Limited</t>
         </is>
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t> </t>
+          <t>3001/252668986/01/000</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2024/07/17</t>
         </is>
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4,56,362.00</t>
         </is>
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7,445.00</t>
         </is>
       </c>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>3,466.00</t>
+          <t>3,716.00</t>
         </is>
       </c>
       <c r="AC25" t="n">
-        <v>3466</v>
+        <v>11161</v>
       </c>
       <c r="AD25" t="n">
-        <v>624</v>
+        <v>2009</v>
       </c>
       <c r="AE25" t="n">
-        <v>4090</v>
+        <v>13170</v>
       </c>
     </row>
     <row r="26">
@@ -4225,27 +4228,28 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>OG-25-1901-1805-00000878</t>
+          <t>OG-25-1901-1801-00002379</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>RAGHAJIBHAI JESHINGBHAI PATEL</t>
+          <t>CHANNAPPA SHIVASHANKAREPPA NIMBAL</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t> </t>
+          <t>8317390500</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>POLICY@TIRTHINSURANCE.COM</t>
+          <t>hiremathsp7@gmail.com</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>PATELFALI, KANPUR,SABARKANTHA,GUJARAT, ,, HIMATNAGAR - 383450</t>
+          <t>S/O SHUVASHANKRAPPA #144, RAMESHWAR COLONY,JAMKHANDI9448035105
+, , BAGALKOT, KARNATAKA-587301</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -4265,77 +4269,77 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>GJ09BB7524</t>
+          <t>KA48M7159</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>GJ09</t>
+          <t>KA48</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>20</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>2014/08/01</t>
+          <t>2015/08/01</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>MARUTI</t>
+          <t>TOYOTA</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>DZIRE</t>
+          <t>INNOVA</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>VDI</t>
+          <t>2.5VX(Diesel)</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>DIESEL</t>
+          <t>Diesel</t>
         </is>
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>D13A2397483</t>
+          <t>556590</t>
         </is>
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>MA3FJEB1S00556058</t>
+          <t>220715</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>1248</t>
+          <t>2494</t>
         </is>
       </c>
       <c r="W26" t="inlineStr">
         <is>
-          <t>Cholamandalam MS General Insurance Company Limited</t>
+          <t>Liberty general insurance limited</t>
         </is>
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>3362/02672321/000/00</t>
+          <t>201150021223700057600000</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
@@ -4345,27 +4349,27 @@
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6,15,000.00</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>9,604.00</t>
         </is>
       </c>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>3,416.00</t>
+          <t>8,347.00</t>
         </is>
       </c>
       <c r="AC26" t="n">
-        <v>3416</v>
+        <v>17951</v>
       </c>
       <c r="AD26" t="n">
-        <v>615</v>
+        <v>3231</v>
       </c>
       <c r="AE26" t="n">
-        <v>4031</v>
+        <v>21182</v>
       </c>
     </row>
     <row r="27">
@@ -4376,146 +4380,902 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>OG-25-1901-1801-00002380</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>GIRISH J M</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>7899365929</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>girishdkj@gmail.com</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>NO 512, 8TH MAIN ROAD 9TH CROSS,SADASHIVANAGAR
+, , BENGALURU, KARNATAKA-560080</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2024/07/17</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024/07/20</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2025/07/19</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>KA04MR9739</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>KA04</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>2016/08/01</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>MARUTI</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>VITARABREZZA</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>1.2ZDIDDIS200</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Diesel</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>D13A5277803</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>MA3NYFB1SGF126243</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>1248</t>
+        </is>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>Future Generali India Insurance Company Limited</t>
+        </is>
+      </c>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>VB999570</t>
+        </is>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>2024/07/19</t>
+        </is>
+      </c>
+      <c r="Z27" t="inlineStr">
+        <is>
+          <t>3,50,000.00</t>
+        </is>
+      </c>
+      <c r="AA27" t="inlineStr">
+        <is>
+          <t>7,582.00</t>
+        </is>
+      </c>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>3,797.00</t>
+        </is>
+      </c>
+      <c r="AC27" t="n">
+        <v>11379</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>2048</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>13427</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Private Car</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>OG-25-1901-1805-00000874</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>JITENDRABHAI MAGANBHAI PATEL</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>mcpatel1985@gmail.com</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>AT-ANIYORKAMPA, TA-MALPUR,DIST-ARVALLI, ,, MALPUR - 383345</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2024/07/17</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024/07/20</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2025/07/19</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>GJ09AG3376</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>GJ09</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>2010/05/01</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>MARUTI</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>RITZ</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>LDI</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>DIESEL</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>D13A1378382</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>MA3FDEB1S00164202</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>1248</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>Future Generali India Insurance Company Limited</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>VB992563</t>
+        </is>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>2024/07/19</t>
+        </is>
+      </c>
+      <c r="Z28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>3,922.00</t>
+        </is>
+      </c>
+      <c r="AC28" t="n">
+        <v>3922</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>706</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>4628</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Private Car</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>OG-25-1901-1805-00000875</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>SARPARIYA NARENDRA VASANTDAS</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>KAPILNIMAVAT93@GMAIL.COM</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>AT, NEAR NEW BUS STAND,UPLETA, ,, RAJKOT - 360490</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2024/07/17</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024/07/19</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2025/07/18</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>GJ25J4484</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>GJ25</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>2015/11/01</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>MARUTI</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>BALENONEW</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>ALPHADIESEL</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>DIESEL</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>D13A2705399</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>MA3EWB62SFK104130</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>1248</t>
+        </is>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Z29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>4,047.00</t>
+        </is>
+      </c>
+      <c r="AC29" t="n">
+        <v>4047</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>728</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>4775</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Private Car</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>OG-25-1901-1805-00000876</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>JAYRAJBHAI AMKUBHAI MANJARIYA</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>mayur_auto02@yahoo.in</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>00, DANEV SOCIETY HANUMAN MANDIR PASE,AT-CHALALA TAL-DHARIDIST-, ,, AMRELI - 365630</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2024/07/17</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024/07/19</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2025/07/18</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>GJ14AK7773</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>GJ14</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>2016/11/01</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>HYUNDAI</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>i20</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>ELITE1.4ASTAU2CRDI6SPEEDMANUALDIESEL</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>DIESEL</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>D4FCGM057507</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>MALBM51RLGM237900</t>
+        </is>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="V30" t="inlineStr">
+        <is>
+          <t>1396</t>
+        </is>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Z30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>3,466.00</t>
+        </is>
+      </c>
+      <c r="AC30" t="n">
+        <v>3466</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>624</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>4090</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Private Car</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>OG-25-1901-1805-00000878</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>RAGHAJIBHAI JESHINGBHAI PATEL</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>POLICY@TIRTHINSURANCE.COM</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>PATELFALI, KANPUR,SABARKANTHA,GUJARAT, ,, HIMATNAGAR - 383450</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2024/07/17</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024/07/20</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2025/07/19</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>GJ09BB7524</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>GJ09</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>2014/08/01</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>MARUTI</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>DZIRE</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>VDI</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>DIESEL</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>D13A2397483</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>MA3FJEB1S00556058</t>
+        </is>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="V31" t="inlineStr">
+        <is>
+          <t>1248</t>
+        </is>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>Cholamandalam MS General Insurance Company Limited</t>
+        </is>
+      </c>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>3362/02672321/000/00</t>
+        </is>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>2024/07/19</t>
+        </is>
+      </c>
+      <c r="Z31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>3,416.00</t>
+        </is>
+      </c>
+      <c r="AC31" t="n">
+        <v>3416</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>615</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>4031</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Private Car</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>OG-25-1901-1805-00000880</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>SOLANKI LATTABEN JAYESHBHAI</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
+      <c r="D32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>POLICY@TIRTHINSURANCE.COM</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>PLOT NO-2379,FLAT NO-14,, RADHESHYAM CPM-PLEX,SUBHASHNAGAR,,GARIADHAR,BHAVNAGAR, ,, BHAVNAGAR - 364001</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>2024/07/17</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>2024/07/19</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>2025/07/18</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="J32" t="inlineStr">
         <is>
           <t>GJ04CJ4212</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr">
+      <c r="K32" t="inlineStr">
         <is>
           <t>GJ04</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
         <is>
           <t>2015/06/01</t>
         </is>
       </c>
-      <c r="N27" t="inlineStr">
+      <c r="N32" t="inlineStr">
         <is>
           <t>FORD</t>
         </is>
       </c>
-      <c r="O27" t="inlineStr">
+      <c r="O32" t="inlineStr">
         <is>
           <t>FIGO</t>
         </is>
       </c>
-      <c r="P27" t="inlineStr">
+      <c r="P32" t="inlineStr">
         <is>
           <t>1.4DURATORQDIESELTITANIUM</t>
         </is>
       </c>
-      <c r="Q27" t="inlineStr">
+      <c r="Q32" t="inlineStr">
         <is>
           <t>2015</t>
         </is>
       </c>
-      <c r="R27" t="inlineStr">
+      <c r="R32" t="inlineStr">
         <is>
           <t>DIESEL</t>
         </is>
       </c>
-      <c r="S27" t="inlineStr">
+      <c r="S32" t="inlineStr">
         <is>
           <t>FE38061</t>
         </is>
       </c>
-      <c r="T27" t="inlineStr">
+      <c r="T32" t="inlineStr">
         <is>
           <t>MAJ1XXMRJ1FE38061</t>
         </is>
       </c>
-      <c r="U27" t="inlineStr">
+      <c r="U32" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="V27" t="inlineStr">
+      <c r="V32" t="inlineStr">
         <is>
           <t>1399</t>
         </is>
       </c>
-      <c r="W27" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="X27" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="Y27" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="Z27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AA27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB27" t="inlineStr">
+      <c r="W32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Z32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB32" t="inlineStr">
         <is>
           <t>4,047.00</t>
         </is>
       </c>
-      <c r="AC27" t="n">
+      <c r="AC32" t="n">
         <v>4047</v>
       </c>
-      <c r="AD27" t="n">
+      <c r="AD32" t="n">
         <v>728</v>
       </c>
-      <c r="AE27" t="n">
+      <c r="AE32" t="n">
         <v>4775</v>
       </c>
     </row>

</xml_diff>